<commit_message>
novo metadados e exemplos de codigo para fazer unpersist de dataframes
</commit_message>
<xml_diff>
--- a/metadados/mapa_das _bases.xlsx
+++ b/metadados/mapa_das _bases.xlsx
@@ -13,12 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="319">
   <si>
     <t>fia_marketing_push</t>
   </si>
   <si>
-    <t>fia_customer_seg</t>
+    <t>fia_customer_segmentation</t>
   </si>
   <si>
     <t>fia_orders</t>
@@ -610,6 +610,9 @@
     <t>De qual feature veio a compra. Se foi de uma lista, de uma busca, ou outro.</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>top_centroid_id</t>
   </si>
   <si>
@@ -628,6 +631,9 @@
     <t>De mídia veio a sessão Google Adwords, Facebook Ads, Twitter</t>
   </si>
   <si>
+    <t>External_user_id</t>
+  </si>
+  <si>
     <t>Data do primeiro pedido.</t>
   </si>
   <si>
@@ -637,6 +643,12 @@
     <t>latitude endereço do usuário (CENTROIDE)</t>
   </si>
   <si>
+    <t>media_attrib_date</t>
+  </si>
+  <si>
+    <t>Data da mídia</t>
+  </si>
+  <si>
     <t>last_order_date</t>
   </si>
   <si>
@@ -649,6 +661,15 @@
     <t>representação do centroide do usuário (concatenado do lat/long do usuário)</t>
   </si>
   <si>
+    <t>chs_fold</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>segmentação de centróides - urbanos de renda alta, média, baixa e não urbanos</t>
+  </si>
+  <si>
     <t>days_to_reorder_at_datasource</t>
   </si>
   <si>
@@ -659,6 +680,12 @@
   </si>
   <si>
     <t>se o usuários tinha serviço de assinatura ativo no momento da compra</t>
+  </si>
+  <si>
+    <t>chs_level</t>
+  </si>
+  <si>
+    <t>Nível do Fold : 1 a 5</t>
   </si>
   <si>
     <t>days_to_reorder_at_concluded</t>
@@ -679,6 +706,12 @@
 Inactive - Não compou no mês anterior nem no retrasado, mas já foi comprador antes</t>
   </si>
   <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Coordenada geográfica captada pelo endereço de entrega registrado, senão houver um endereço registrado, será captado a posição do dispositivo.</t>
+  </si>
+  <si>
     <t>rfv_score</t>
   </si>
   <si>
@@ -686,9 +719,6 @@
   </si>
   <si>
     <t>customer_seg_recency_bucket</t>
-  </si>
-  <si>
-    <t>int</t>
   </si>
   <si>
     <t>bucket referente a quão próximo foi feita a última compra:
@@ -699,6 +729,9 @@
 1 - Último pedido há mais de 91 dias</t>
   </si>
   <si>
+    <t>longitude</t>
+  </si>
+  <si>
     <t>recency_days</t>
   </si>
   <si>
@@ -716,6 +749,12 @@
 1 - Menos que 1 pedido/mês</t>
   </si>
   <si>
+    <t>event_start_at_amsp</t>
+  </si>
+  <si>
+    <t>Data e hora de inicío do evento</t>
+  </si>
+  <si>
     <t>recency_days_bucket</t>
   </si>
   <si>
@@ -733,6 +772,15 @@
 1 - Até 21 reais</t>
   </si>
   <si>
+    <t>dt_amsp timestamp</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>baseada no fuso América/São Paulo</t>
+  </si>
+  <si>
     <t>recency_days_bucket_description</t>
   </si>
   <si>
@@ -748,6 +796,12 @@
 3 - Entre 90 e 150 restaurantes
 2 - Entre 30 e 90 restaurantes
 1 - Até 30 restaurantes</t>
+  </si>
+  <si>
+    <t>dt_partition</t>
+  </si>
+  <si>
+    <t>Coluna de particionamento</t>
   </si>
   <si>
     <t>freq_last_91d</t>
@@ -939,12 +993,6 @@
     <t>quantidade dos itens promocionados (promo_is_promotion = 1)</t>
   </si>
   <si>
-    <t>media_attrib_date</t>
-  </si>
-  <si>
-    <t>Data da mídia</t>
-  </si>
-  <si>
     <t>merchant_offer_bucket_description</t>
   </si>
   <si>
@@ -957,12 +1005,6 @@
     <t>diferença entre o dia do pedido e o dia do pedido anterior</t>
   </si>
   <si>
-    <t>chs_fold</t>
-  </si>
-  <si>
-    <t>segmentação de centróides - urbanos de renda alta, média, baixa e não urbanos</t>
-  </si>
-  <si>
     <t>top_dish_bucket</t>
   </si>
   <si>
@@ -975,12 +1017,6 @@
     <t>diferença entre o dia do pedido e o dia do próximo pedido</t>
   </si>
   <si>
-    <t>chs_level</t>
-  </si>
-  <si>
-    <t>Nível do Fold : 1 a 5</t>
-  </si>
-  <si>
     <t>top_dish_bucket_description</t>
   </si>
   <si>
@@ -993,12 +1029,6 @@
     <t>diferença entre o mês do pedido e o mês do próximo pedido</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>Coordenada geográfica captada pelo endereço de entrega registrado, senão houver um endereço registrado, será captado a posição do dispositivo.</t>
-  </si>
-  <si>
     <t>preferred_dishes</t>
   </si>
   <si>
@@ -1011,9 +1041,6 @@
     <t>diferença entre o mês do pedido e o mês do pedido anterior</t>
   </si>
   <si>
-    <t>longitude</t>
-  </si>
-  <si>
     <t>preferred_dishes_code</t>
   </si>
   <si>
@@ -1021,27 +1048,6 @@
   </si>
   <si>
     <t>data do pedido</t>
-  </si>
-  <si>
-    <t>event_start_at_amsp</t>
-  </si>
-  <si>
-    <t>Data e hora de inicío do evento</t>
-  </si>
-  <si>
-    <t>dt_amsp timestamp</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>baseada no fuso América/São Paulo</t>
-  </si>
-  <si>
-    <t>dt_partition</t>
-  </si>
-  <si>
-    <t>Coluna de particionamento</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -1155,11 +1161,30 @@
         <color rgb="FF000000"/>
       </left>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1201,6 +1226,12 @@
     </xf>
     <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -1441,9 +1472,10 @@
     <col customWidth="1" min="3" max="3" width="45.29"/>
     <col customWidth="1" min="5" max="5" width="34.29"/>
     <col customWidth="1" min="7" max="7" width="51.0"/>
-    <col customWidth="1" min="8" max="8" width="10.71"/>
-    <col customWidth="1" min="9" max="9" width="36.71"/>
-    <col customWidth="1" min="11" max="11" width="52.57"/>
+    <col customWidth="1" hidden="1" min="8" max="8" width="10.71"/>
+    <col customWidth="1" hidden="1" min="9" max="9" width="36.71"/>
+    <col hidden="1" min="10" max="10" width="14.43"/>
+    <col customWidth="1" hidden="1" min="11" max="11" width="52.57"/>
     <col customWidth="1" min="13" max="13" width="40.14"/>
     <col customWidth="1" min="15" max="15" width="43.71"/>
     <col customWidth="1" min="17" max="17" width="26.86"/>
@@ -2629,28 +2661,34 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" ht="22.5" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>185</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2658,13 +2696,13 @@
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R23" s="12" t="s">
         <v>9</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
@@ -2675,9 +2713,15 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" ht="22.5" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>185</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="8" t="s">
         <v>44</v>
@@ -2686,23 +2730,32 @@
         <v>9</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
+      <c r="Q24" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="R24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2717,29 +2770,38 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="8" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="8" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
+      <c r="Q25" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="S25" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -2754,29 +2816,38 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="8" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="8" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>115</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
+      <c r="Q26" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -2791,29 +2862,38 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="8" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="8" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
+      <c r="Q27" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="R27" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>216</v>
+      </c>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -2828,29 +2908,38 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="8" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="8" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
+      <c r="Q28" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="R28" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S28" s="10" t="s">
+        <v>216</v>
+      </c>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -2865,29 +2954,38 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="8" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="8" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
+      <c r="Q29" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="R29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="S29" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
@@ -2902,29 +3000,38 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="8" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="8" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
+      <c r="Q30" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="R30" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="S30" s="10" t="s">
+        <v>234</v>
+      </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
@@ -2939,29 +3046,38 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="8" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="8" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
+      <c r="Q31" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="R31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S31" s="10" t="s">
+        <v>240</v>
+      </c>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
@@ -2976,23 +3092,23 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="8" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="8" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="14" t="s">
-        <v>226</v>
+      <c r="K32" s="16" t="s">
+        <v>244</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -3013,23 +3129,23 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="8" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="8" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -3050,23 +3166,23 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="8" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="8" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -3087,23 +3203,23 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="8" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="8" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -3124,13 +3240,13 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="8" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>40</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="8" t="s">
@@ -3140,16 +3256,16 @@
         <v>9</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="15"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="17"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -3164,32 +3280,32 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="8" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="8" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="17"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="19"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
@@ -3204,32 +3320,32 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="8" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="8" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="15"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="17"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -3244,32 +3360,32 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="8" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="8" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="17"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="19"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
@@ -3284,32 +3400,32 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="8" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="8" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="J40" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="16"/>
-      <c r="S40" s="15"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="17"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -3324,32 +3440,32 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="8" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="8" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="17"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="19"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
@@ -3364,32 +3480,32 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="8" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="8" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="15"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="17"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
@@ -3404,32 +3520,32 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="8" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="8" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="21"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
@@ -3444,32 +3560,32 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="8" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="8" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="16"/>
-      <c r="S44" s="15"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="17"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
@@ -3484,23 +3600,23 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="8" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>40</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="8" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
@@ -3521,38 +3637,29 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="8" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="8" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="J46" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
-      <c r="Q46" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="R46" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="S46" s="15" t="s">
-        <v>283</v>
-      </c>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
@@ -3567,38 +3674,29 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="8" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="8" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="Q47" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="R47" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="S47" s="17" t="s">
-        <v>289</v>
-      </c>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
@@ -3613,38 +3711,29 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="8" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>120</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="8" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-      <c r="Q48" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="R48" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="S48" s="15" t="s">
-        <v>295</v>
-      </c>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
@@ -3659,38 +3748,29 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="8" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="8" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="Q49" s="17" t="s">
-        <v>300</v>
-      </c>
-      <c r="R49" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="S49" s="17" t="s">
-        <v>301</v>
-      </c>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
@@ -3705,38 +3785,29 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="8" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>147</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="8" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="R50" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="S50" s="15" t="s">
-        <v>301</v>
-      </c>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
@@ -3751,13 +3822,13 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="8" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>147</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="8" t="s">
@@ -3767,22 +3838,13 @@
         <v>9</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-      <c r="Q51" s="17" t="s">
-        <v>310</v>
-      </c>
-      <c r="R51" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="S51" s="17" t="s">
-        <v>311</v>
-      </c>
       <c r="T51" s="3"/>
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
@@ -3796,7 +3858,7 @@
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="20"/>
+      <c r="E52" s="22"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -3805,15 +3867,6 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
-      <c r="Q52" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="R52" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="S52" s="15" t="s">
-        <v>314</v>
-      </c>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -3839,15 +3892,6 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-      <c r="Q53" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="R53" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="S53" s="17" t="s">
-        <v>316</v>
-      </c>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>

</xml_diff>